<commit_message>
27-09-2023_00 measure unities corrected + notebook created
</commit_message>
<xml_diff>
--- a/kinectic-modeling/data/fastpetase-fig6-analisada_EXCEL.xlsx
+++ b/kinectic-modeling/data/fastpetase-fig6-analisada_EXCEL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\root\Estudos\Institucional\UNILA\iGEM\drylab_unila_repository\kinectic-modeling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{729C4038-975F-4202-9889-F10F99B5781A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F19CC79-E061-4558-AA1E-4D76948B1CCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -208,10 +208,10 @@
     <t>taxa (mg/dia)</t>
   </si>
   <si>
-    <t>quantidade enzima purificada (nM)</t>
-  </si>
-  <si>
     <t>degradação mg/diaM</t>
+  </si>
+  <si>
+    <t>quantidade enzima purificada (uM)</t>
   </si>
 </sst>
 </file>
@@ -611,23 +611,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A6:X63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.5546875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.77734375" style="2" customWidth="1"/>
     <col min="3" max="3" width="22.44140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="21.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="38.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.44140625" style="2" customWidth="1"/>
-    <col min="7" max="24" width="13.5546875" style="2"/>
+    <col min="6" max="7" width="13.5546875" style="2"/>
+    <col min="9" max="24" width="13.5546875" style="2"/>
     <col min="25" max="16384" width="13.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>54</v>
       </c>
@@ -635,7 +635,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="4" t="s">
         <v>51</v>
@@ -647,16 +647,16 @@
         <v>56</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
       <c r="X7" s="1"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>34</v>
       </c>
@@ -671,17 +671,17 @@
         <v>1.2105263157894737</v>
       </c>
       <c r="E8" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F8" s="2">
         <f>D8/E8</f>
-        <v>6.0526315789473685E-3</v>
+        <v>6.0526315789473681</v>
       </c>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
       <c r="X8" s="1"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>50</v>
       </c>
@@ -696,17 +696,17 @@
         <v>1.842857142857143</v>
       </c>
       <c r="E9" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F9" s="2">
-        <f t="shared" ref="F9:F59" si="1">D9/E9</f>
-        <v>9.2142857142857148E-3</v>
+        <f>D9/E9</f>
+        <v>9.2142857142857135</v>
       </c>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>48</v>
       </c>
@@ -721,17 +721,17 @@
         <v>1.9402985074626866</v>
       </c>
       <c r="E10" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F10" s="2">
-        <f t="shared" si="1"/>
-        <v>9.7014925373134324E-3</v>
+        <f>D10/E10</f>
+        <v>9.7014925373134329</v>
       </c>
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>24</v>
       </c>
@@ -746,17 +746,17 @@
         <v>2.4666666666666668</v>
       </c>
       <c r="E11" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F11" s="2">
-        <f t="shared" si="1"/>
-        <v>1.2333333333333333E-2</v>
+        <f>D11/E11</f>
+        <v>12.333333333333334</v>
       </c>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>37</v>
       </c>
@@ -771,17 +771,17 @@
         <v>2.6341463414634152</v>
       </c>
       <c r="E12" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F12" s="2">
-        <f t="shared" si="1"/>
-        <v>1.3170731707317076E-2</v>
+        <f>D12/E12</f>
+        <v>13.170731707317076</v>
       </c>
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>46</v>
       </c>
@@ -796,17 +796,17 @@
         <v>2.6346153846153846</v>
       </c>
       <c r="E13" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F13" s="2">
-        <f t="shared" si="1"/>
-        <v>1.3173076923076923E-2</v>
+        <f>D13/E13</f>
+        <v>13.173076923076922</v>
       </c>
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>28</v>
       </c>
@@ -821,17 +821,17 @@
         <v>2.7647058823529416</v>
       </c>
       <c r="E14" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F14" s="2">
-        <f t="shared" si="1"/>
-        <v>1.3823529411764708E-2</v>
+        <f>D14/E14</f>
+        <v>13.823529411764707</v>
       </c>
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>40</v>
       </c>
@@ -846,17 +846,17 @@
         <v>2.8636363636363633</v>
       </c>
       <c r="E15" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F15" s="2">
-        <f t="shared" si="1"/>
-        <v>1.4318181818181817E-2</v>
+        <f>D15/E15</f>
+        <v>14.318181818181817</v>
       </c>
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>11</v>
       </c>
@@ -871,17 +871,17 @@
         <v>2.88</v>
       </c>
       <c r="E16" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F16" s="2">
-        <f t="shared" si="1"/>
-        <v>1.44E-2</v>
+        <f>D16/E16</f>
+        <v>14.399999999999999</v>
       </c>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>19</v>
       </c>
@@ -896,17 +896,17 @@
         <v>2.896551724137931</v>
       </c>
       <c r="E17" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F17" s="2">
-        <f t="shared" si="1"/>
-        <v>1.4482758620689656E-2</v>
+        <f>D17/E17</f>
+        <v>14.482758620689655</v>
       </c>
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
       <c r="X17" s="1"/>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>29</v>
       </c>
@@ -921,17 +921,17 @@
         <v>2.9459459459459461</v>
       </c>
       <c r="E18" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F18" s="2">
-        <f t="shared" si="1"/>
-        <v>1.472972972972973E-2</v>
+        <f>D18/E18</f>
+        <v>14.72972972972973</v>
       </c>
       <c r="V18" s="1"/>
       <c r="W18" s="1"/>
       <c r="X18" s="1"/>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>31</v>
       </c>
@@ -946,17 +946,17 @@
         <v>2.9459459459459461</v>
       </c>
       <c r="E19" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F19" s="2">
-        <f t="shared" si="1"/>
-        <v>1.472972972972973E-2</v>
+        <f>D19/E19</f>
+        <v>14.72972972972973</v>
       </c>
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
       <c r="X19" s="1"/>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
         <v>36</v>
       </c>
@@ -971,17 +971,17 @@
         <v>2.9487179487179489</v>
       </c>
       <c r="E20" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F20" s="2">
-        <f t="shared" si="1"/>
-        <v>1.4743589743589745E-2</v>
+        <f>D20/E20</f>
+        <v>14.743589743589745</v>
       </c>
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
       <c r="X20" s="1"/>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
         <v>38</v>
       </c>
@@ -996,17 +996,17 @@
         <v>2.9761904761904763</v>
       </c>
       <c r="E21" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F21" s="2">
-        <f t="shared" si="1"/>
-        <v>1.4880952380952382E-2</v>
+        <f>D21/E21</f>
+        <v>14.880952380952381</v>
       </c>
       <c r="V21" s="1"/>
       <c r="W21" s="1"/>
       <c r="X21" s="1"/>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>43</v>
       </c>
@@ -1021,17 +1021,17 @@
         <v>2.978723404255319</v>
       </c>
       <c r="E22" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F22" s="2">
-        <f t="shared" si="1"/>
-        <v>1.4893617021276595E-2</v>
+        <f>D22/E22</f>
+        <v>14.893617021276594</v>
       </c>
       <c r="V22" s="1"/>
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>1</v>
       </c>
@@ -1046,17 +1046,17 @@
         <v>3</v>
       </c>
       <c r="E23" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F23" s="2">
-        <f t="shared" si="1"/>
-        <v>1.4999999999999999E-2</v>
+        <f>D23/E23</f>
+        <v>15</v>
       </c>
       <c r="V23" s="1"/>
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>16</v>
       </c>
@@ -1071,17 +1071,17 @@
         <v>3.0000000000000004</v>
       </c>
       <c r="E24" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F24" s="2">
-        <f t="shared" si="1"/>
-        <v>1.5000000000000003E-2</v>
+        <f>D24/E24</f>
+        <v>15.000000000000002</v>
       </c>
       <c r="V24" s="1"/>
       <c r="W24" s="1"/>
       <c r="X24" s="1"/>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>8</v>
       </c>
@@ -1096,17 +1096,17 @@
         <v>3.0434782608695654</v>
       </c>
       <c r="E25" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F25" s="2">
-        <f t="shared" si="1"/>
-        <v>1.5217391304347827E-2</v>
+        <f>D25/E25</f>
+        <v>15.217391304347826</v>
       </c>
       <c r="V25" s="1"/>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
         <v>3</v>
       </c>
@@ -1121,17 +1121,17 @@
         <v>3.05</v>
       </c>
       <c r="E26" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F26" s="2">
-        <f t="shared" si="1"/>
-        <v>1.525E-2</v>
+        <f>D26/E26</f>
+        <v>15.249999999999998</v>
       </c>
       <c r="V26" s="1"/>
       <c r="W26" s="1"/>
       <c r="X26" s="1"/>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
         <v>32</v>
       </c>
@@ -1146,17 +1146,17 @@
         <v>3.0789473684210527</v>
       </c>
       <c r="E27" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F27" s="2">
-        <f t="shared" si="1"/>
-        <v>1.5394736842105263E-2</v>
+        <f>D27/E27</f>
+        <v>15.394736842105262</v>
       </c>
       <c r="V27" s="1"/>
       <c r="W27" s="1"/>
       <c r="X27" s="1"/>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>41</v>
       </c>
@@ -1171,17 +1171,17 @@
         <v>3.0869565217391304</v>
       </c>
       <c r="E28" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F28" s="2">
-        <f t="shared" si="1"/>
-        <v>1.5434782608695652E-2</v>
+        <f>D28/E28</f>
+        <v>15.434782608695651</v>
       </c>
       <c r="V28" s="1"/>
       <c r="W28" s="1"/>
       <c r="X28" s="1"/>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
         <v>33</v>
       </c>
@@ -1196,17 +1196,17 @@
         <v>3.1315789473684212</v>
       </c>
       <c r="E29" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F29" s="2">
-        <f t="shared" si="1"/>
-        <v>1.5657894736842107E-2</v>
+        <f>D29/E29</f>
+        <v>15.657894736842106</v>
       </c>
       <c r="V29" s="1"/>
       <c r="W29" s="1"/>
       <c r="X29" s="1"/>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
         <v>17</v>
       </c>
@@ -1221,17 +1221,17 @@
         <v>3.1428571428571432</v>
       </c>
       <c r="E30" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F30" s="2">
-        <f t="shared" si="1"/>
-        <v>1.5714285714285715E-2</v>
+        <f>D30/E30</f>
+        <v>15.714285714285715</v>
       </c>
       <c r="V30" s="1"/>
       <c r="W30" s="1"/>
       <c r="X30" s="1"/>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>49</v>
       </c>
@@ -1246,17 +1246,17 @@
         <v>3.1764705882352944</v>
       </c>
       <c r="E31" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F31" s="2">
-        <f t="shared" si="1"/>
-        <v>1.5882352941176472E-2</v>
+        <f>D31/E31</f>
+        <v>15.882352941176471</v>
       </c>
       <c r="V31" s="1"/>
       <c r="W31" s="1"/>
       <c r="X31" s="1"/>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
         <v>30</v>
       </c>
@@ -1271,17 +1271,17 @@
         <v>3.2162162162162162</v>
       </c>
       <c r="E32" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F32" s="2">
-        <f t="shared" si="1"/>
-        <v>1.608108108108108E-2</v>
+        <f>D32/E32</f>
+        <v>16.081081081081081</v>
       </c>
       <c r="V32" s="1"/>
       <c r="W32" s="1"/>
       <c r="X32" s="1"/>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
         <v>42</v>
       </c>
@@ -1296,17 +1296,17 @@
         <v>3.2608695652173916</v>
       </c>
       <c r="E33" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F33" s="2">
-        <f t="shared" si="1"/>
-        <v>1.630434782608696E-2</v>
+        <f>D33/E33</f>
+        <v>16.304347826086957</v>
       </c>
       <c r="V33" s="1"/>
       <c r="W33" s="1"/>
       <c r="X33" s="1"/>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
         <v>22</v>
       </c>
@@ -1321,17 +1321,17 @@
         <v>3.2758620689655173</v>
       </c>
       <c r="E34" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F34" s="2">
-        <f t="shared" si="1"/>
-        <v>1.6379310344827588E-2</v>
+        <f>D34/E34</f>
+        <v>16.379310344827587</v>
       </c>
       <c r="V34" s="1"/>
       <c r="W34" s="1"/>
       <c r="X34" s="1"/>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>35</v>
       </c>
@@ -1346,17 +1346,17 @@
         <v>3.2820512820512824</v>
       </c>
       <c r="E35" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F35" s="2">
-        <f t="shared" si="1"/>
-        <v>1.641025641025641E-2</v>
+        <f>D35/E35</f>
+        <v>16.410256410256412</v>
       </c>
       <c r="V35" s="1"/>
       <c r="W35" s="1"/>
       <c r="X35" s="1"/>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
         <v>18</v>
       </c>
@@ -1371,17 +1371,17 @@
         <v>3.2857142857142856</v>
       </c>
       <c r="E36" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F36" s="2">
-        <f t="shared" si="1"/>
-        <v>1.6428571428571428E-2</v>
+        <f>D36/E36</f>
+        <v>16.428571428571427</v>
       </c>
       <c r="V36" s="1"/>
       <c r="W36" s="1"/>
       <c r="X36" s="1"/>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
         <v>12</v>
       </c>
@@ -1396,17 +1396,17 @@
         <v>3.3076923076923075</v>
       </c>
       <c r="E37" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F37" s="2">
-        <f t="shared" si="1"/>
-        <v>1.6538461538461537E-2</v>
+        <f>D37/E37</f>
+        <v>16.538461538461537</v>
       </c>
       <c r="V37" s="1"/>
       <c r="W37" s="1"/>
       <c r="X37" s="1"/>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
         <v>21</v>
       </c>
@@ -1421,17 +1421,17 @@
         <v>3.3103448275862069</v>
       </c>
       <c r="E38" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F38" s="2">
-        <f t="shared" si="1"/>
-        <v>1.6551724137931035E-2</v>
+        <f>D38/E38</f>
+        <v>16.551724137931032</v>
       </c>
       <c r="V38" s="1"/>
       <c r="W38" s="1"/>
       <c r="X38" s="1"/>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
         <v>26</v>
       </c>
@@ -1446,17 +1446,17 @@
         <v>3.3124999999999996</v>
       </c>
       <c r="E39" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F39" s="2">
-        <f t="shared" si="1"/>
-        <v>1.6562499999999997E-2</v>
+        <f>D39/E39</f>
+        <v>16.562499999999996</v>
       </c>
       <c r="V39" s="1"/>
       <c r="W39" s="1"/>
       <c r="X39" s="1"/>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
         <v>47</v>
       </c>
@@ -1467,21 +1467,21 @@
         <v>20.3</v>
       </c>
       <c r="D40" s="2">
-        <f t="shared" ref="D40:D71" si="2">C40/B40</f>
+        <f t="shared" ref="D40:D58" si="1">C40/B40</f>
         <v>3.3278688524590168</v>
       </c>
       <c r="E40" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F40" s="2">
-        <f t="shared" si="1"/>
-        <v>1.6639344262295085E-2</v>
+        <f>D40/E40</f>
+        <v>16.639344262295083</v>
       </c>
       <c r="V40" s="1"/>
       <c r="W40" s="1"/>
       <c r="X40" s="1"/>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
         <v>45</v>
       </c>
@@ -1492,21 +1492,21 @@
         <v>17.100000000000001</v>
       </c>
       <c r="D41" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.3529411764705888</v>
       </c>
       <c r="E41" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F41" s="2">
-        <f t="shared" si="1"/>
-        <v>1.6764705882352945E-2</v>
+        <f>D41/E41</f>
+        <v>16.764705882352942</v>
       </c>
       <c r="V41" s="1"/>
       <c r="W41" s="1"/>
       <c r="X41" s="1"/>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
         <v>44</v>
       </c>
@@ -1517,21 +1517,21 @@
         <v>16.100000000000001</v>
       </c>
       <c r="D42" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.354166666666667</v>
       </c>
       <c r="E42" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F42" s="2">
-        <f t="shared" si="1"/>
-        <v>1.6770833333333336E-2</v>
+        <f>D42/E42</f>
+        <v>16.770833333333332</v>
       </c>
       <c r="V42" s="1"/>
       <c r="W42" s="1"/>
       <c r="X42" s="1"/>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
         <v>15</v>
       </c>
@@ -1542,21 +1542,21 @@
         <v>9.1</v>
       </c>
       <c r="D43" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.3703703703703702</v>
       </c>
       <c r="E43" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F43" s="2">
-        <f t="shared" si="1"/>
-        <v>1.6851851851851851E-2</v>
+        <f>D43/E43</f>
+        <v>16.851851851851851</v>
       </c>
       <c r="V43" s="1"/>
       <c r="W43" s="1"/>
       <c r="X43" s="1"/>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
         <v>27</v>
       </c>
@@ -1567,21 +1567,21 @@
         <v>10.9</v>
       </c>
       <c r="D44" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.40625</v>
       </c>
       <c r="E44" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F44" s="2">
-        <f t="shared" si="1"/>
-        <v>1.7031250000000001E-2</v>
+        <f>D44/E44</f>
+        <v>17.03125</v>
       </c>
       <c r="V44" s="1"/>
       <c r="W44" s="1"/>
       <c r="X44" s="1"/>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
         <v>2</v>
       </c>
@@ -1592,21 +1592,21 @@
         <v>6.5</v>
       </c>
       <c r="D45" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.4210526315789473</v>
       </c>
       <c r="E45" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F45" s="2">
-        <f t="shared" si="1"/>
-        <v>1.7105263157894738E-2</v>
+        <f>D45/E45</f>
+        <v>17.105263157894736</v>
       </c>
       <c r="V45" s="1"/>
       <c r="W45" s="1"/>
       <c r="X45" s="1"/>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
         <v>14</v>
       </c>
@@ -1617,21 +1617,21 @@
         <v>9</v>
       </c>
       <c r="D46" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.4615384615384612</v>
       </c>
       <c r="E46" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F46" s="2">
-        <f t="shared" si="1"/>
-        <v>1.7307692307692305E-2</v>
+        <f>D46/E46</f>
+        <v>17.307692307692307</v>
       </c>
       <c r="V46" s="1"/>
       <c r="W46" s="1"/>
       <c r="X46" s="1"/>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
         <v>10</v>
       </c>
@@ -1642,21 +1642,21 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="D47" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.5200000000000005</v>
       </c>
       <c r="E47" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F47" s="2">
-        <f t="shared" si="1"/>
-        <v>1.7600000000000001E-2</v>
+        <f>D47/E47</f>
+        <v>17.600000000000001</v>
       </c>
       <c r="V47" s="1"/>
       <c r="W47" s="1"/>
       <c r="X47" s="1"/>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
         <v>39</v>
       </c>
@@ -1667,21 +1667,21 @@
         <v>14.9</v>
       </c>
       <c r="D48" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.5476190476190474</v>
       </c>
       <c r="E48" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F48" s="2">
-        <f t="shared" si="1"/>
-        <v>1.7738095238095237E-2</v>
+        <f>D48/E48</f>
+        <v>17.738095238095237</v>
       </c>
       <c r="V48" s="1"/>
       <c r="W48" s="1"/>
       <c r="X48" s="1"/>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
         <v>6</v>
       </c>
@@ -1692,21 +1692,21 @@
         <v>7.5</v>
       </c>
       <c r="D49" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.5714285714285712</v>
       </c>
       <c r="E49" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F49" s="2">
-        <f t="shared" si="1"/>
-        <v>1.7857142857142856E-2</v>
+        <f>D49/E49</f>
+        <v>17.857142857142854</v>
       </c>
       <c r="V49" s="1"/>
       <c r="W49" s="1"/>
       <c r="X49" s="1"/>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
         <v>13</v>
       </c>
@@ -1717,21 +1717,21 @@
         <v>9.4</v>
       </c>
       <c r="D50" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.6153846153846154</v>
       </c>
       <c r="E50" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F50" s="2">
-        <f t="shared" si="1"/>
-        <v>1.8076923076923077E-2</v>
+        <f>D50/E50</f>
+        <v>18.076923076923077</v>
       </c>
       <c r="V50" s="1"/>
       <c r="W50" s="1"/>
       <c r="X50" s="1"/>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
         <v>20</v>
       </c>
@@ -1742,21 +1742,21 @@
         <v>10.6</v>
       </c>
       <c r="D51" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.6551724137931036</v>
       </c>
       <c r="E51" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F51" s="2">
-        <f t="shared" si="1"/>
-        <v>1.8275862068965518E-2</v>
+        <f>D51/E51</f>
+        <v>18.275862068965516</v>
       </c>
       <c r="V51" s="1"/>
       <c r="W51" s="1"/>
       <c r="X51" s="1"/>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
         <v>23</v>
       </c>
@@ -1767,21 +1767,21 @@
         <v>11</v>
       </c>
       <c r="D52" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.6666666666666665</v>
       </c>
       <c r="E52" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F52" s="2">
-        <f t="shared" si="1"/>
-        <v>1.8333333333333333E-2</v>
+        <f>D52/E52</f>
+        <v>18.333333333333332</v>
       </c>
       <c r="V52" s="1"/>
       <c r="W52" s="1"/>
       <c r="X52" s="1"/>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A53" s="6" t="s">
         <v>5</v>
       </c>
@@ -1792,21 +1792,21 @@
         <v>7.9</v>
       </c>
       <c r="D53" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.7619047619047619</v>
       </c>
       <c r="E53" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F53" s="2">
-        <f t="shared" si="1"/>
-        <v>1.8809523809523811E-2</v>
+        <f>D53/E53</f>
+        <v>18.809523809523807</v>
       </c>
       <c r="V53" s="1"/>
       <c r="W53" s="1"/>
       <c r="X53" s="1"/>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
         <v>25</v>
       </c>
@@ -1817,21 +1817,21 @@
         <v>11.5</v>
       </c>
       <c r="D54" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.8333333333333335</v>
       </c>
       <c r="E54" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F54" s="2">
-        <f t="shared" si="1"/>
-        <v>1.9166666666666669E-2</v>
+        <f>D54/E54</f>
+        <v>19.166666666666668</v>
       </c>
       <c r="V54" s="1"/>
       <c r="W54" s="1"/>
       <c r="X54" s="1"/>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
         <v>4</v>
       </c>
@@ -1842,21 +1842,21 @@
         <v>8.1</v>
       </c>
       <c r="D55" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.8571428571428568</v>
       </c>
       <c r="E55" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F55" s="2">
-        <f t="shared" si="1"/>
-        <v>1.9285714285714285E-2</v>
+        <f>D55/E55</f>
+        <v>19.285714285714281</v>
       </c>
       <c r="V55" s="1"/>
       <c r="W55" s="1"/>
       <c r="X55" s="1"/>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
         <v>7</v>
       </c>
@@ -1867,21 +1867,21 @@
         <v>8.5</v>
       </c>
       <c r="D56" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.8636363636363633</v>
       </c>
       <c r="E56" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F56" s="2">
-        <f t="shared" si="1"/>
-        <v>1.9318181818181818E-2</v>
+        <f>D56/E56</f>
+        <v>19.318181818181817</v>
       </c>
       <c r="V56" s="1"/>
       <c r="W56" s="1"/>
       <c r="X56" s="1"/>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
         <v>9</v>
       </c>
@@ -1892,21 +1892,21 @@
         <v>8.9</v>
       </c>
       <c r="D57" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3.8695652173913047</v>
       </c>
       <c r="E57" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F57" s="2">
-        <f t="shared" si="1"/>
-        <v>1.9347826086956524E-2</v>
+        <f>D57/E57</f>
+        <v>19.347826086956523</v>
       </c>
       <c r="V57" s="1"/>
       <c r="W57" s="1"/>
       <c r="X57" s="1"/>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
         <v>0</v>
       </c>
@@ -1917,21 +1917,21 @@
         <v>6.7</v>
       </c>
       <c r="D58" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6.7</v>
       </c>
       <c r="E58" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F58" s="2">
-        <f t="shared" si="1"/>
-        <v>3.3500000000000002E-2</v>
+        <f>D58/E58</f>
+        <v>33.5</v>
       </c>
       <c r="V58" s="1"/>
       <c r="W58" s="1"/>
       <c r="X58" s="1"/>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C59" s="2" t="s">
         <v>55</v>
       </c>
@@ -1940,14 +1940,14 @@
         <v>3.1417604828695249</v>
       </c>
       <c r="E59" s="2">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="F59" s="2">
-        <f t="shared" si="1"/>
-        <v>1.5708802414347623E-2</v>
-      </c>
-    </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
+        <f>D59/E59</f>
+        <v>15.708802414347623</v>
+      </c>
+    </row>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
       <c r="X63" s="1"/>
     </row>
   </sheetData>

</xml_diff>